<commit_message>
add additional cleaning function
</commit_message>
<xml_diff>
--- a/data/poas/poas17.xlsx
+++ b/data/poas/poas17.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaime/Desktop/poas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64FB99D-02EB-5242-AA70-241A5026FD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB157437-2EBA-2A40-A6DF-4E14D2A435DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,8 +535,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
@@ -1218,7 +1218,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="28" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="28" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
@@ -1259,13 +1259,13 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="10" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1713,7 +1713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U433"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
@@ -29895,19 +29895,61 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="d7a46b7f-bbdc-422f-b9e0-20b6fc8455c0">KNWUJA4RVW4F-197578868-7978</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="d7a46b7f-bbdc-422f-b9e0-20b6fc8455c0">
-      <Url>https://recruiting.rsn.army.mil/mrb/SORB/_layouts/15/DocIdRedir.aspx?ID=KNWUJA4RVW4F-197578868-7978</Url>
-      <Description>KNWUJA4RVW4F-197578868-7978</Description>
-    </_dlc_DocIdUrl>
-    <Content1 xmlns="b35d94ff-169f-4fda-be0e-711916431615">FOUO</Content1>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E9CFC2744C53CC4A903B5B4AF3029F9A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="97ee4e959f82058e0960f3436bd440fa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b35d94ff-169f-4fda-be0e-711916431615" xmlns:ns3="d7a46b7f-bbdc-422f-b9e0-20b6fc8455c0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0533c712f566362aefb0b1437ef461a6" ns2:_="" ns3:_="">
     <xsd:import namespace="b35d94ff-169f-4fda-be0e-711916431615"/>
@@ -30086,73 +30128,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="d7a46b7f-bbdc-422f-b9e0-20b6fc8455c0">KNWUJA4RVW4F-197578868-7978</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="d7a46b7f-bbdc-422f-b9e0-20b6fc8455c0">
+      <Url>https://recruiting.rsn.army.mil/mrb/SORB/_layouts/15/DocIdRedir.aspx?ID=KNWUJA4RVW4F-197578868-7978</Url>
+      <Description>KNWUJA4RVW4F-197578868-7978</Description>
+    </_dlc_DocIdUrl>
+    <Content1 xmlns="b35d94ff-169f-4fda-be0e-711916431615">FOUO</Content1>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666BB67B-E4EB-45EE-AFA6-8E6AD957F47D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E03627-00E4-4246-84FB-2A4FD54756F9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d7a46b7f-bbdc-422f-b9e0-20b6fc8455c0"/>
-    <ds:schemaRef ds:uri="b35d94ff-169f-4fda-be0e-711916431615"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{349052E8-CBD5-4583-824C-B57042717E2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F409FD3B-67BB-473B-AD8F-652F146BAFE6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30171,18 +30176,13 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{349052E8-CBD5-4583-824C-B57042717E2B}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666BB67B-E4EB-45EE-AFA6-8E6AD957F47D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E03627-00E4-4246-84FB-2A4FD54756F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d7a46b7f-bbdc-422f-b9e0-20b6fc8455c0"/>
+    <ds:schemaRef ds:uri="b35d94ff-169f-4fda-be0e-711916431615"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>